<commit_message>
new excel sheet format
</commit_message>
<xml_diff>
--- a/data/POS_2025_03_backup.xlsx
+++ b/data/POS_2025_03_backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\Desktop\www\Python\Al_Halal_POS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED50E16B-C1EF-4CE2-9A75-A49E66B3A4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A6F31-1D2C-450B-8C82-F8C26A9B3EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,12 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
   <si>
     <t>Item Name</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Inventory Quantity</t>
   </si>
   <si>
     <t>Quantity Sold</t>
@@ -53,22 +59,22 @@
     <t>Sale Price</t>
   </si>
   <si>
-    <t>Inventory Quantity</t>
-  </si>
-  <si>
-    <t>Barcode</t>
+    <t>Total Profit</t>
+  </si>
+  <si>
+    <t>Invested</t>
+  </si>
+  <si>
+    <t>Clean Profit</t>
   </si>
   <si>
     <t>Kurt Ermak</t>
   </si>
   <si>
-    <t>Invested</t>
-  </si>
-  <si>
-    <t>Clean Profit</t>
-  </si>
-  <si>
-    <t>Total Profit</t>
+    <t>WL0047968</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,6 +160,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,45 +479,45 @@
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1"/>
@@ -521,17 +530,17 @@
         <v>4780022250220</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E2" s="3">
         <v>100</v>
       </c>
       <c r="F2" s="3">
         <f>D2-E2</f>
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="G2" s="4">
         <v>2500</v>
@@ -545,25 +554,48 @@
       </c>
       <c r="J2" s="2">
         <f>D2*G2</f>
-        <v>250000</v>
+        <v>220000</v>
       </c>
       <c r="K2" s="2">
         <f>I2-J2</f>
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="G3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I25" si="0">H3*E3</f>
+        <v>100000</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J25" si="1">D3*G3</f>
+        <v>100000</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K25" si="2">I3-J3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -574,9 +606,20 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -587,9 +630,20 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -600,9 +654,20 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -613,9 +678,20 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -626,9 +702,20 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -639,9 +726,20 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -652,9 +750,20 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -663,9 +772,216 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>